<commit_message>
update report for finace
</commit_message>
<xml_diff>
--- a/ACCOUNT_REPORT/Source/WISOL.UI/FINANCING_STATEMENT.xlsx
+++ b/ACCOUNT_REPORT/Source/WISOL.UI/FINANCING_STATEMENT.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$A$1:$H$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$A$1:$H$49</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -294,21 +294,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="12">
+  <numFmts count="9">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-&quot;₩&quot;* #,##0_-;\-&quot;₩&quot;* #,##0_-;_-&quot;₩&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="\$#,##0.00"/>
     <numFmt numFmtId="167" formatCode="\$#,##0.00;[Red]\-\$#,##0.00"/>
     <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,10 +493,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
+      <sz val="10"/>
+      <name val="맑은 고딕"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
     </font>
   </fonts>
   <fills count="5">
@@ -528,7 +529,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -634,146 +635,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -796,21 +657,6 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -1004,202 +850,61 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
+      <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
@@ -1216,622 +921,525 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="14" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="14" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="38" fontId="14" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="14" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="0" xfId="8" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="14" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="14" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="14" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="14" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="25" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="26" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="25" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="25" fillId="4" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="23" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="14" fillId="2" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="22" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="14" fillId="2" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="14" fillId="4" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="14" fillId="2" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="2" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="7" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="2" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="2" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="14" fillId="2" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="22" fillId="2" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="22" fillId="2" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="22" fillId="2" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="2" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="22" fillId="2" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="22" fillId="2" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="22" fillId="2" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="2" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="17" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="23" fillId="4" borderId="18" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="17" fillId="2" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="2" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="2" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="2" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="2" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="22" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="29" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="29" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="14" fillId="2" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="22" fillId="4" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="2" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="29" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="26" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="29" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="29" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="2" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="14" fillId="4" borderId="24" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="14" fillId="2" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="2" borderId="34" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="8" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="28" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="2" borderId="35" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="2" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="29" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="14" fillId="2" borderId="24" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="14" fillId="2" borderId="24" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="2" borderId="28" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="2" borderId="28" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="2" borderId="28" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="2" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="2" borderId="29" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="2" borderId="30" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="2" borderId="28" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="22" fillId="2" borderId="35" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="17" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="23" fillId="4" borderId="29" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="17" fillId="2" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="14" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="14" fillId="2" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="4" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="4" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="27" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="27" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="25" fillId="0" borderId="43" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="26" fillId="4" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="25" fillId="4" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="2" borderId="32" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="2" borderId="35" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="25" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="26" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="21" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="14" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="14" fillId="2" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="22" fillId="2" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="22" fillId="2" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+  <cellStyles count="8">
+    <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="쉼표 [0] 2" xfId="4"/>
-    <cellStyle name="쉼표 [0] 3" xfId="7"/>
-    <cellStyle name="쉼표 [0] 3 2 2" xfId="5"/>
-    <cellStyle name="표준 2" xfId="3"/>
-    <cellStyle name="표준 3 2 2" xfId="8"/>
-    <cellStyle name="표준_자금0206" xfId="6"/>
+    <cellStyle name="쉼표 [0] 2" xfId="3"/>
+    <cellStyle name="쉼표 [0] 3" xfId="6"/>
+    <cellStyle name="쉼표 [0] 3 2 2" xfId="4"/>
+    <cellStyle name="표준 2" xfId="2"/>
+    <cellStyle name="표준 3 2 2" xfId="7"/>
+    <cellStyle name="표준_자금0206" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2112,10 +1720,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:AH249"/>
+  <dimension ref="A1:AH243"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.5"/>
@@ -2582,125 +2190,125 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" ht="24" customHeight="1">
-      <c r="A2" s="184" t="s">
+      <c r="A2" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="184"/>
-      <c r="D2" s="184"/>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
-      <c r="H2" s="185"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="153"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="186" t="s">
+      <c r="A3" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="186"/>
-      <c r="C3" s="186"/>
-      <c r="D3" s="186"/>
-      <c r="E3" s="186"/>
-      <c r="F3" s="186"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="187"/>
+      <c r="B3" s="154"/>
+      <c r="C3" s="154"/>
+      <c r="D3" s="154"/>
+      <c r="E3" s="154"/>
+      <c r="F3" s="154"/>
+      <c r="G3" s="154"/>
+      <c r="H3" s="155"/>
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="77"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="79"/>
+      <c r="H4" s="54"/>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="80"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="82" t="s">
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="83" t="s">
+      <c r="H5" s="58" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="84"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="188" t="s">
+      <c r="A6" s="59"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="156" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="191"/>
-      <c r="H6" s="194"/>
+      <c r="G6" s="159"/>
+      <c r="H6" s="162"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1">
-      <c r="A7" s="84"/>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="189"/>
-      <c r="G7" s="192"/>
-      <c r="H7" s="195"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="157"/>
+      <c r="G7" s="160"/>
+      <c r="H7" s="163"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="190"/>
-      <c r="G8" s="193"/>
-      <c r="H8" s="196"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="158"/>
+      <c r="G8" s="161"/>
+      <c r="H8" s="164"/>
     </row>
     <row r="9" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="144" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
+      <c r="B9" s="144"/>
+      <c r="C9" s="144"/>
+      <c r="D9" s="144"/>
       <c r="E9" s="14"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
-      <c r="H9" s="87"/>
+      <c r="H9" s="61"/>
     </row>
     <row r="10" spans="1:9" ht="26.45" customHeight="1" thickBot="1">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="62" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="88" t="s">
+      <c r="D10" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="89" t="s">
+      <c r="E10" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="89" t="s">
+      <c r="F10" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="89" t="s">
+      <c r="G10" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="90" t="s">
+      <c r="H10" s="64" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2709,41 +2317,41 @@
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
+      <c r="E11" s="118"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
-      <c r="H11" s="91"/>
+      <c r="H11" s="65"/>
     </row>
     <row r="12" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A12" s="92"/>
-      <c r="B12" s="92"/>
-      <c r="C12" s="93"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="95"/>
-      <c r="F12" s="95"/>
-      <c r="G12" s="96"/>
-      <c r="H12" s="97"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="69"/>
     </row>
     <row r="13" spans="1:9" ht="26.45" customHeight="1">
-      <c r="A13" s="197" t="s">
+      <c r="A13" s="147" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="198"/>
-      <c r="C13" s="183"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98">
-        <f>SUM(E12:E12)</f>
+      <c r="B13" s="148"/>
+      <c r="C13" s="149"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70">
+        <f>SUM(E11:E12)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="98">
-        <f>SUM(F12:F12)</f>
+      <c r="F13" s="70">
+        <f>SUM(F11:F12)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="99">
-        <f>SUM(G12:G12)</f>
+      <c r="G13" s="71">
+        <f>SUM(G11:G12)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="100"/>
+      <c r="H13" s="72"/>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1">
       <c r="A14" s="12"/>
@@ -2753,15 +2361,15 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="101"/>
+      <c r="H14" s="73"/>
     </row>
     <row r="15" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A15" s="199" t="s">
+      <c r="A15" s="144" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="199"/>
-      <c r="C15" s="199"/>
-      <c r="D15" s="199"/>
+      <c r="B15" s="144"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="144"/>
       <c r="E15" s="20" t="s">
         <v>14</v>
       </c>
@@ -2771,7 +2379,7 @@
       <c r="G15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="102"/>
+      <c r="H15" s="74"/>
     </row>
     <row r="16" spans="1:9" ht="20.25" customHeight="1" thickBot="1">
       <c r="A16" s="22" t="s">
@@ -2795,7 +2403,7 @@
       <c r="G16" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="103" t="s">
+      <c r="H16" s="75" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2803,45 +2411,48 @@
       <c r="A17" s="24"/>
       <c r="B17" s="25"/>
       <c r="C17" s="26"/>
-      <c r="D17" s="104"/>
-      <c r="E17" s="104"/>
-      <c r="F17" s="104"/>
-      <c r="G17" s="104"/>
-      <c r="H17" s="105"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="77"/>
       <c r="I17" s="27"/>
       <c r="J17" s="28"/>
     </row>
     <row r="18" spans="1:11" ht="20.25" customHeight="1">
-      <c r="A18" s="106"/>
-      <c r="B18" s="107"/>
-      <c r="C18" s="108"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="104"/>
-      <c r="G18" s="104"/>
-      <c r="H18" s="109"/>
+      <c r="A18" s="78"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="81"/>
       <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:11" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A19" s="181" t="s">
+      <c r="A19" s="150" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="182"/>
-      <c r="C19" s="183"/>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110">
+      <c r="B19" s="151"/>
+      <c r="C19" s="149"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82">
         <f t="shared" ref="E19:G19" si="0">SUM(E17:E18)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="110">
+      <c r="F19" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="110">
+      <c r="G19" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H19" s="111"/>
+      <c r="H19" s="83" t="e">
+        <f>G19/H20</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="20" spans="1:11" s="10" customFormat="1" ht="19.5" customHeight="1">
       <c r="A20" s="12"/>
@@ -2853,31 +2464,29 @@
       <c r="G20" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="112">
-        <v>23000</v>
-      </c>
+      <c r="H20" s="84"/>
       <c r="I20" s="32"/>
     </row>
     <row r="21" spans="1:11" s="10" customFormat="1" ht="21" customHeight="1">
-      <c r="A21" s="199" t="s">
+      <c r="A21" s="144" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="199"/>
-      <c r="C21" s="199"/>
+      <c r="B21" s="144"/>
+      <c r="C21" s="144"/>
       <c r="D21" s="13"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="33"/>
-      <c r="H21" s="113"/>
+      <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:11" s="10" customFormat="1" ht="21" customHeight="1" thickBot="1">
-      <c r="A22" s="114" t="s">
+      <c r="A22" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="114" t="s">
+      <c r="B22" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="114" t="s">
+      <c r="C22" s="86" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="34" t="s">
@@ -2892,7 +2501,7 @@
       <c r="G22" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="115" t="s">
+      <c r="H22" s="87" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2900,44 +2509,44 @@
       <c r="A23" s="37"/>
       <c r="B23" s="38"/>
       <c r="C23" s="39"/>
-      <c r="D23" s="104"/>
-      <c r="E23" s="104"/>
-      <c r="F23" s="104"/>
-      <c r="G23" s="104"/>
-      <c r="H23" s="116"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="88"/>
       <c r="I23" s="40"/>
     </row>
     <row r="24" spans="1:11" s="10" customFormat="1" ht="21" customHeight="1">
-      <c r="A24" s="117"/>
-      <c r="B24" s="118"/>
-      <c r="C24" s="119"/>
-      <c r="D24" s="104"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="104"/>
-      <c r="G24" s="104"/>
-      <c r="H24" s="120"/>
+      <c r="A24" s="89"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="92"/>
       <c r="I24" s="41"/>
     </row>
     <row r="25" spans="1:11" s="10" customFormat="1" ht="21" customHeight="1">
-      <c r="A25" s="181" t="s">
+      <c r="A25" s="150" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="182"/>
-      <c r="C25" s="183"/>
-      <c r="D25" s="121"/>
-      <c r="E25" s="121">
+      <c r="B25" s="151"/>
+      <c r="C25" s="149"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="93">
         <f t="shared" ref="E25:G25" si="1">SUM(E23:E24)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="121">
+      <c r="F25" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G25" s="99">
+      <c r="G25" s="71">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H25" s="122"/>
+      <c r="H25" s="94"/>
     </row>
     <row r="26" spans="1:11" s="10" customFormat="1" ht="21" customHeight="1">
       <c r="A26" s="12"/>
@@ -2947,20 +2556,20 @@
       <c r="E26" s="42"/>
       <c r="F26" s="19"/>
       <c r="G26" s="43"/>
-      <c r="H26" s="123"/>
+      <c r="H26" s="95"/>
       <c r="I26" s="44"/>
     </row>
     <row r="27" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A27" s="124" t="s">
+      <c r="A27" s="143" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
+      <c r="B27" s="143"/>
+      <c r="C27" s="143"/>
       <c r="D27" s="13"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
-      <c r="G27" s="200"/>
-      <c r="H27" s="201"/>
+      <c r="G27" s="145"/>
+      <c r="H27" s="146"/>
       <c r="J27" s="29"/>
     </row>
     <row r="28" spans="1:11" ht="20.25" customHeight="1" thickBot="1">
@@ -2985,7 +2594,7 @@
       <c r="G28" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="103" t="s">
+      <c r="H28" s="75" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2993,40 +2602,40 @@
       <c r="A29" s="45"/>
       <c r="B29" s="46"/>
       <c r="C29" s="47"/>
-      <c r="D29" s="104"/>
-      <c r="E29" s="104"/>
-      <c r="F29" s="104"/>
-      <c r="G29" s="104"/>
-      <c r="H29" s="125"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="96"/>
       <c r="J29" s="30"/>
       <c r="K29" s="31"/>
     </row>
     <row r="30" spans="1:11" ht="20.25" customHeight="1">
-      <c r="A30" s="126"/>
-      <c r="B30" s="107"/>
-      <c r="C30" s="108"/>
-      <c r="D30" s="104"/>
-      <c r="E30" s="104"/>
-      <c r="F30" s="104"/>
-      <c r="G30" s="104"/>
-      <c r="H30" s="125"/>
+      <c r="A30" s="97"/>
+      <c r="B30" s="79"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="96"/>
       <c r="J30" s="30"/>
       <c r="K30" s="31"/>
     </row>
     <row r="31" spans="1:11" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A31" s="181"/>
-      <c r="B31" s="182"/>
-      <c r="C31" s="183"/>
-      <c r="D31" s="110">
+      <c r="A31" s="150"/>
+      <c r="B31" s="151"/>
+      <c r="C31" s="149"/>
+      <c r="D31" s="82">
         <f>SUM(D29:D30)</f>
         <v>0</v>
       </c>
-      <c r="E31" s="110"/>
-      <c r="F31" s="110"/>
-      <c r="G31" s="98"/>
-      <c r="H31" s="111">
-        <f>D41/H32</f>
-        <v>0</v>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="83" t="e">
+        <f>D31/H32</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="10" customFormat="1" ht="19.5" customHeight="1">
@@ -3039,117 +2648,114 @@
       <c r="G32" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H32" s="127">
-        <f>H20</f>
-        <v>23000</v>
-      </c>
+      <c r="H32" s="84"/>
     </row>
     <row r="33" spans="1:34" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A33" s="178" t="s">
+      <c r="A33" s="167" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="178"/>
-      <c r="C33" s="178"/>
+      <c r="B33" s="167"/>
+      <c r="C33" s="167"/>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
-      <c r="H33" s="128"/>
+      <c r="H33" s="98"/>
     </row>
     <row r="34" spans="1:34" s="27" customFormat="1" ht="21" customHeight="1">
-      <c r="A34" s="129" t="s">
+      <c r="A34" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="130" t="s">
+      <c r="B34" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="130" t="s">
+      <c r="C34" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="131" t="s">
+      <c r="D34" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="132" t="s">
+      <c r="E34" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="133" t="s">
+      <c r="F34" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="G34" s="179" t="s">
+      <c r="G34" s="168" t="s">
         <v>13</v>
       </c>
-      <c r="H34" s="180"/>
+      <c r="H34" s="169"/>
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:34" s="27" customFormat="1" ht="21" customHeight="1">
-      <c r="A35" s="129"/>
-      <c r="B35" s="134"/>
-      <c r="C35" s="134"/>
-      <c r="D35" s="104"/>
-      <c r="E35" s="104"/>
-      <c r="F35" s="104"/>
-      <c r="G35" s="135"/>
-      <c r="H35" s="136"/>
+      <c r="A35" s="99"/>
+      <c r="B35" s="104"/>
+      <c r="C35" s="104"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="105"/>
+      <c r="H35" s="106"/>
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:34" s="27" customFormat="1" ht="21" customHeight="1">
-      <c r="A36" s="129"/>
-      <c r="B36" s="134"/>
-      <c r="C36" s="134"/>
-      <c r="D36" s="104"/>
-      <c r="E36" s="104"/>
-      <c r="F36" s="104"/>
-      <c r="G36" s="137"/>
-      <c r="H36" s="138"/>
+      <c r="A36" s="99"/>
+      <c r="B36" s="104"/>
+      <c r="C36" s="104"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="107"/>
+      <c r="H36" s="108"/>
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:34" s="27" customFormat="1" ht="21" customHeight="1">
-      <c r="A37" s="129"/>
-      <c r="B37" s="139"/>
-      <c r="C37" s="139"/>
-      <c r="D37" s="104">
+      <c r="A37" s="99"/>
+      <c r="B37" s="109"/>
+      <c r="C37" s="109"/>
+      <c r="D37" s="76">
         <f>SUM(D35:D36)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="104">
+      <c r="E37" s="76">
         <f t="shared" ref="E37:G37" si="2">SUM(E35:E36)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="104">
+      <c r="F37" s="76">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G37" s="104">
+      <c r="G37" s="76">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H37" s="138"/>
+      <c r="H37" s="108"/>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="1:34" s="27" customFormat="1" ht="24" customHeight="1">
-      <c r="A38" s="140"/>
-      <c r="B38" s="140"/>
-      <c r="C38" s="140"/>
-      <c r="D38" s="140"/>
-      <c r="E38" s="141"/>
-      <c r="F38" s="142" t="s">
+    <row r="38" spans="1:34" s="27" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A38" s="110"/>
+      <c r="B38" s="110"/>
+      <c r="C38" s="110"/>
+      <c r="D38" s="110"/>
+      <c r="E38" s="111"/>
+      <c r="F38" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="G38" s="143"/>
-      <c r="H38" s="144"/>
+      <c r="G38" s="113"/>
+      <c r="H38" s="114"/>
       <c r="I38" s="48"/>
     </row>
-    <row r="39" spans="1:34" s="49" customFormat="1" ht="21" customHeight="1" thickBot="1">
-      <c r="A39" s="145" t="s">
+    <row r="39" spans="1:34" s="49" customFormat="1" ht="21" customHeight="1">
+      <c r="A39" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="146"/>
-      <c r="C39" s="146"/>
-      <c r="D39" s="146"/>
-      <c r="E39" s="146"/>
-      <c r="F39" s="146"/>
-      <c r="G39" s="146"/>
-      <c r="H39" s="147"/>
+      <c r="B39" s="116"/>
+      <c r="C39" s="116"/>
+      <c r="D39" s="116"/>
+      <c r="E39" s="116"/>
+      <c r="F39" s="116"/>
+      <c r="G39" s="116"/>
+      <c r="H39" s="117"/>
       <c r="R39" s="27"/>
       <c r="S39" s="27"/>
       <c r="T39" s="27"/>
@@ -3168,29 +2774,29 @@
       <c r="AG39" s="27"/>
       <c r="AH39" s="27"/>
     </row>
-    <row r="40" spans="1:34" s="50" customFormat="1" ht="14.25" thickBot="1">
-      <c r="A40" s="51" t="s">
+    <row r="40" spans="1:34" s="50" customFormat="1" ht="18" customHeight="1">
+      <c r="A40" s="141" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="141" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="52" t="s">
+      <c r="C40" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="52" t="s">
+      <c r="D40" s="141" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="52" t="s">
+      <c r="E40" s="141" t="s">
         <v>43</v>
       </c>
-      <c r="F40" s="52" t="s">
+      <c r="F40" s="141" t="s">
         <v>44</v>
       </c>
-      <c r="G40" s="52" t="s">
+      <c r="G40" s="141" t="s">
         <v>45</v>
       </c>
-      <c r="H40" s="53" t="s">
+      <c r="H40" s="142" t="s">
         <v>46</v>
       </c>
       <c r="I40" s="49"/>
@@ -3220,17 +2826,17 @@
       <c r="AG40" s="27"/>
       <c r="AH40" s="27"/>
     </row>
-    <row r="41" spans="1:34" s="50" customFormat="1" ht="15">
-      <c r="A41" s="54" t="s">
+    <row r="41" spans="1:34" s="50" customFormat="1" ht="18" customHeight="1">
+      <c r="A41" s="123" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="55"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="57"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="148"/>
+      <c r="B41" s="124"/>
+      <c r="C41" s="139"/>
+      <c r="D41" s="125"/>
+      <c r="E41" s="140"/>
+      <c r="F41" s="121"/>
+      <c r="G41" s="121"/>
+      <c r="H41" s="122"/>
       <c r="I41" s="49"/>
       <c r="J41" s="49"/>
       <c r="K41" s="49"/>
@@ -3258,15 +2864,15 @@
       <c r="AG41" s="27"/>
       <c r="AH41" s="27"/>
     </row>
-    <row r="42" spans="1:34" s="50" customFormat="1" ht="15">
-      <c r="A42" s="59"/>
-      <c r="B42" s="149"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="150"/>
-      <c r="H42" s="151"/>
+    <row r="42" spans="1:34" s="50" customFormat="1" ht="18" customHeight="1">
+      <c r="A42" s="123"/>
+      <c r="B42" s="126"/>
+      <c r="C42" s="127"/>
+      <c r="D42" s="126"/>
+      <c r="E42" s="136"/>
+      <c r="F42" s="120"/>
+      <c r="G42" s="120"/>
+      <c r="H42" s="119"/>
       <c r="I42" s="49"/>
       <c r="J42" s="49"/>
       <c r="K42" s="49"/>
@@ -3294,15 +2900,25 @@
       <c r="AG42" s="27"/>
       <c r="AH42" s="27"/>
     </row>
-    <row r="43" spans="1:34" s="50" customFormat="1" ht="15">
-      <c r="A43" s="152"/>
-      <c r="B43" s="153"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="154"/>
-      <c r="F43" s="154"/>
-      <c r="G43" s="155"/>
-      <c r="H43" s="156"/>
+    <row r="43" spans="1:34" s="50" customFormat="1" ht="18" customHeight="1">
+      <c r="A43" s="165" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="129"/>
+      <c r="C43" s="130"/>
+      <c r="D43" s="129"/>
+      <c r="E43" s="131" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" s="132">
+        <f>+SUMIF($E$41:$E$42,$E43,$F$41:$F$42)</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="132">
+        <f>+SUMIF($E$41:$E$42,$E43,$G$41:$G$42)</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="133"/>
       <c r="I43" s="49"/>
       <c r="J43" s="49"/>
       <c r="K43" s="49"/>
@@ -3330,15 +2946,23 @@
       <c r="AG43" s="27"/>
       <c r="AH43" s="27"/>
     </row>
-    <row r="44" spans="1:34" s="50" customFormat="1" ht="14.25" thickBot="1">
-      <c r="A44" s="157"/>
-      <c r="B44" s="158"/>
-      <c r="C44" s="159"/>
-      <c r="D44" s="158"/>
-      <c r="E44" s="158"/>
-      <c r="F44" s="158"/>
-      <c r="G44" s="158"/>
-      <c r="H44" s="160"/>
+    <row r="44" spans="1:34" s="50" customFormat="1" ht="18" customHeight="1">
+      <c r="A44" s="166"/>
+      <c r="B44" s="129"/>
+      <c r="C44" s="130"/>
+      <c r="D44" s="129"/>
+      <c r="E44" s="131" t="s">
+        <v>50</v>
+      </c>
+      <c r="F44" s="132">
+        <f>+SUMIF($E$41:$E$42,$E44,$F$41:$F$42)</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="132">
+        <f>+SUMIF($E$41:$E$42,$E44,$G$41:$G$42)</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="133"/>
       <c r="I44" s="49"/>
       <c r="J44" s="49"/>
       <c r="K44" s="49"/>
@@ -3366,25 +2990,17 @@
       <c r="AG44" s="27"/>
       <c r="AH44" s="27"/>
     </row>
-    <row r="45" spans="1:34" s="50" customFormat="1">
-      <c r="A45" s="173" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="62"/>
-      <c r="C45" s="62"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="F45" s="62">
-        <f>+SUMIF($E$41:$E$44,$E45,$F$41:$F$44)</f>
-        <v>0</v>
-      </c>
-      <c r="G45" s="64">
-        <f>+SUMIF($E$41:$E$44,$E45,$G$41:$G$44)</f>
-        <v>0</v>
-      </c>
-      <c r="H45" s="161"/>
+    <row r="45" spans="1:34" s="50" customFormat="1" ht="18" customHeight="1">
+      <c r="A45" s="128" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="124"/>
+      <c r="C45" s="128"/>
+      <c r="D45" s="124"/>
+      <c r="E45" s="137"/>
+      <c r="F45" s="121"/>
+      <c r="G45" s="121"/>
+      <c r="H45" s="122"/>
       <c r="I45" s="49"/>
       <c r="J45" s="49"/>
       <c r="K45" s="49"/>
@@ -3412,23 +3028,15 @@
       <c r="AG45" s="27"/>
       <c r="AH45" s="27"/>
     </row>
-    <row r="46" spans="1:34" s="50" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A46" s="174"/>
-      <c r="B46" s="65"/>
-      <c r="C46" s="162"/>
-      <c r="D46" s="162"/>
-      <c r="E46" s="163" t="s">
-        <v>50</v>
-      </c>
-      <c r="F46" s="162">
-        <f>+SUMIF($E$41:$E$44,$E46,$F$41:$F$44)</f>
-        <v>0</v>
-      </c>
-      <c r="G46" s="164">
-        <f>+SUMIF($E$41:$E$44,$E46,$G$41:$G$44)</f>
-        <v>0</v>
-      </c>
-      <c r="H46" s="165"/>
+    <row r="46" spans="1:34" s="50" customFormat="1" ht="18" customHeight="1">
+      <c r="A46" s="123"/>
+      <c r="B46" s="126"/>
+      <c r="C46" s="123"/>
+      <c r="D46" s="126"/>
+      <c r="E46" s="138"/>
+      <c r="F46" s="120"/>
+      <c r="G46" s="120"/>
+      <c r="H46" s="119"/>
       <c r="I46" s="49"/>
       <c r="J46" s="49"/>
       <c r="K46" s="49"/>
@@ -3456,17 +3064,25 @@
       <c r="AG46" s="27"/>
       <c r="AH46" s="27"/>
     </row>
-    <row r="47" spans="1:34" s="50" customFormat="1">
-      <c r="A47" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="175"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="57"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="66"/>
+    <row r="47" spans="1:34" s="50" customFormat="1" ht="18" customHeight="1">
+      <c r="A47" s="165" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="134"/>
+      <c r="C47" s="135"/>
+      <c r="D47" s="134"/>
+      <c r="E47" s="131" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="132">
+        <f>+SUMIF($E$45:$E$46,$E47,$F$45:$F$46)</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="132">
+        <f>+SUMIF($E$45:$E$46,$E47,$G$45:$G$46)</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="133"/>
       <c r="I47" s="49"/>
       <c r="J47" s="49"/>
       <c r="K47" s="49"/>
@@ -3494,15 +3110,23 @@
       <c r="AG47" s="27"/>
       <c r="AH47" s="27"/>
     </row>
-    <row r="48" spans="1:34" s="50" customFormat="1">
-      <c r="A48" s="59"/>
-      <c r="B48" s="176"/>
-      <c r="C48" s="67"/>
-      <c r="D48" s="68"/>
-      <c r="E48" s="68"/>
-      <c r="F48" s="68"/>
-      <c r="G48" s="69"/>
-      <c r="H48" s="70"/>
+    <row r="48" spans="1:34" s="50" customFormat="1" ht="18" customHeight="1">
+      <c r="A48" s="166"/>
+      <c r="B48" s="134"/>
+      <c r="C48" s="135"/>
+      <c r="D48" s="134"/>
+      <c r="E48" s="131" t="s">
+        <v>50</v>
+      </c>
+      <c r="F48" s="132">
+        <f>+SUMIF($E$45:$E$46,$E48,$F$45:$F$46)</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="132">
+        <f>+SUMIF($E$45:$E$46,$E48,$G$45:$G$46)</f>
+        <v>0</v>
+      </c>
+      <c r="H48" s="133"/>
       <c r="I48" s="49"/>
       <c r="J48" s="49"/>
       <c r="K48" s="49"/>
@@ -3530,15 +3154,7 @@
       <c r="AG48" s="27"/>
       <c r="AH48" s="27"/>
     </row>
-    <row r="49" spans="1:34" s="50" customFormat="1">
-      <c r="A49" s="59"/>
-      <c r="B49" s="176"/>
-      <c r="C49" s="67"/>
-      <c r="D49" s="68"/>
-      <c r="E49" s="68"/>
-      <c r="F49" s="68"/>
-      <c r="G49" s="69"/>
-      <c r="H49" s="70"/>
+    <row r="49" spans="9:34" s="50" customFormat="1">
       <c r="I49" s="49"/>
       <c r="J49" s="49"/>
       <c r="K49" s="49"/>
@@ -3566,243 +3182,23 @@
       <c r="AG49" s="27"/>
       <c r="AH49" s="27"/>
     </row>
-    <row r="50" spans="1:34" s="50" customFormat="1">
-      <c r="A50" s="59"/>
-      <c r="B50" s="177"/>
-      <c r="C50" s="67"/>
-      <c r="D50" s="68"/>
-      <c r="E50" s="68"/>
-      <c r="F50" s="68"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="49"/>
-      <c r="J50" s="49"/>
-      <c r="K50" s="49"/>
-      <c r="L50" s="49"/>
-      <c r="M50" s="49"/>
-      <c r="N50" s="49"/>
-      <c r="O50" s="49"/>
-      <c r="P50" s="49"/>
-      <c r="Q50" s="49"/>
-      <c r="R50" s="27"/>
-      <c r="S50" s="27"/>
-      <c r="T50" s="27"/>
-      <c r="U50" s="27"/>
-      <c r="V50" s="27"/>
-      <c r="W50" s="27"/>
-      <c r="X50" s="27"/>
-      <c r="Y50" s="27"/>
-      <c r="Z50" s="27"/>
-      <c r="AA50" s="27"/>
-      <c r="AB50" s="27"/>
-      <c r="AC50" s="27"/>
-      <c r="AD50" s="27"/>
-      <c r="AE50" s="27"/>
-      <c r="AF50" s="27"/>
-      <c r="AG50" s="27"/>
-      <c r="AH50" s="27"/>
-    </row>
-    <row r="51" spans="1:34" s="50" customFormat="1">
-      <c r="A51" s="59"/>
-      <c r="B51" s="166"/>
-      <c r="C51" s="60"/>
-      <c r="D51" s="61"/>
-      <c r="E51" s="61"/>
-      <c r="F51" s="61"/>
-      <c r="G51" s="71"/>
-      <c r="H51" s="72"/>
-      <c r="I51" s="49"/>
-      <c r="J51" s="49"/>
-      <c r="K51" s="49"/>
-      <c r="L51" s="49"/>
-      <c r="M51" s="49"/>
-      <c r="N51" s="49"/>
-      <c r="O51" s="49"/>
-      <c r="P51" s="49"/>
-      <c r="Q51" s="49"/>
-      <c r="R51" s="27"/>
-      <c r="S51" s="27"/>
-      <c r="T51" s="27"/>
-      <c r="U51" s="27"/>
-      <c r="V51" s="27"/>
-      <c r="W51" s="27"/>
-      <c r="X51" s="27"/>
-      <c r="Y51" s="27"/>
-      <c r="Z51" s="27"/>
-      <c r="AA51" s="27"/>
-      <c r="AB51" s="27"/>
-      <c r="AC51" s="27"/>
-      <c r="AD51" s="27"/>
-      <c r="AE51" s="27"/>
-      <c r="AF51" s="27"/>
-      <c r="AG51" s="27"/>
-      <c r="AH51" s="27"/>
-    </row>
-    <row r="52" spans="1:34" s="50" customFormat="1" ht="14.25" thickBot="1">
-      <c r="A52" s="167"/>
-      <c r="B52" s="168"/>
-      <c r="C52" s="168"/>
-      <c r="D52" s="168"/>
-      <c r="E52" s="168"/>
-      <c r="F52" s="168"/>
-      <c r="G52" s="168"/>
-      <c r="H52" s="169"/>
-      <c r="I52" s="49"/>
-      <c r="J52" s="49"/>
-      <c r="K52" s="49"/>
-      <c r="L52" s="49"/>
-      <c r="M52" s="49"/>
-      <c r="N52" s="49"/>
-      <c r="O52" s="49"/>
-      <c r="P52" s="49"/>
-      <c r="Q52" s="49"/>
-      <c r="R52" s="27"/>
-      <c r="S52" s="27"/>
-      <c r="T52" s="27"/>
-      <c r="U52" s="27"/>
-      <c r="V52" s="27"/>
-      <c r="W52" s="27"/>
-      <c r="X52" s="27"/>
-      <c r="Y52" s="27"/>
-      <c r="Z52" s="27"/>
-      <c r="AA52" s="27"/>
-      <c r="AB52" s="27"/>
-      <c r="AC52" s="27"/>
-      <c r="AD52" s="27"/>
-      <c r="AE52" s="27"/>
-      <c r="AF52" s="27"/>
-      <c r="AG52" s="27"/>
-      <c r="AH52" s="27"/>
-    </row>
-    <row r="53" spans="1:34" s="50" customFormat="1">
-      <c r="A53" s="173" t="s">
-        <v>52</v>
-      </c>
-      <c r="B53" s="73"/>
-      <c r="C53" s="73"/>
-      <c r="D53" s="73"/>
-      <c r="E53" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="F53" s="74">
-        <f>+SUMIF($E$47:$E$52,$E53,$F$47:$F$52)</f>
-        <v>0</v>
-      </c>
-      <c r="G53" s="74">
-        <f>+SUMIF($E$47:$E$52,$E53,$G$47:$G$52)</f>
-        <v>0</v>
-      </c>
-      <c r="H53" s="75"/>
-      <c r="I53" s="49"/>
-      <c r="J53" s="49"/>
-      <c r="K53" s="49"/>
-      <c r="L53" s="49"/>
-      <c r="M53" s="49"/>
-      <c r="N53" s="49"/>
-      <c r="O53" s="49"/>
-      <c r="P53" s="49"/>
-      <c r="Q53" s="49"/>
-      <c r="R53" s="27"/>
-      <c r="S53" s="27"/>
-      <c r="T53" s="27"/>
-      <c r="U53" s="27"/>
-      <c r="V53" s="27"/>
-      <c r="W53" s="27"/>
-      <c r="X53" s="27"/>
-      <c r="Y53" s="27"/>
-      <c r="Z53" s="27"/>
-      <c r="AA53" s="27"/>
-      <c r="AB53" s="27"/>
-      <c r="AC53" s="27"/>
-      <c r="AD53" s="27"/>
-      <c r="AE53" s="27"/>
-      <c r="AF53" s="27"/>
-      <c r="AG53" s="27"/>
-      <c r="AH53" s="27"/>
-    </row>
-    <row r="54" spans="1:34" s="50" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A54" s="174"/>
-      <c r="B54" s="170"/>
-      <c r="C54" s="170"/>
-      <c r="D54" s="170"/>
-      <c r="E54" s="163" t="s">
-        <v>50</v>
-      </c>
-      <c r="F54" s="171">
-        <f>+SUMIF($E$47:$E$52,$E54,$F$47:$F$52)</f>
-        <v>0</v>
-      </c>
-      <c r="G54" s="171">
-        <f>+SUMIF($E$47:$E$52,$E54,$G$47:$G$52)</f>
-        <v>0</v>
-      </c>
-      <c r="H54" s="172"/>
-      <c r="I54" s="49"/>
-      <c r="J54" s="49"/>
-      <c r="K54" s="49"/>
-      <c r="L54" s="49"/>
-      <c r="M54" s="49"/>
-      <c r="N54" s="49"/>
-      <c r="O54" s="49"/>
-      <c r="P54" s="49"/>
-      <c r="Q54" s="49"/>
-      <c r="R54" s="27"/>
-      <c r="S54" s="27"/>
-      <c r="T54" s="27"/>
-      <c r="U54" s="27"/>
-      <c r="V54" s="27"/>
-      <c r="W54" s="27"/>
-      <c r="X54" s="27"/>
-      <c r="Y54" s="27"/>
-      <c r="Z54" s="27"/>
-      <c r="AA54" s="27"/>
-      <c r="AB54" s="27"/>
-      <c r="AC54" s="27"/>
-      <c r="AD54" s="27"/>
-      <c r="AE54" s="27"/>
-      <c r="AF54" s="27"/>
-      <c r="AG54" s="27"/>
-      <c r="AH54" s="27"/>
-    </row>
-    <row r="55" spans="1:34" s="50" customFormat="1">
-      <c r="I55" s="49"/>
-      <c r="J55" s="49"/>
-      <c r="K55" s="49"/>
-      <c r="L55" s="49"/>
-      <c r="M55" s="49"/>
-      <c r="N55" s="49"/>
-      <c r="O55" s="49"/>
-      <c r="P55" s="49"/>
-      <c r="Q55" s="49"/>
-      <c r="R55" s="27"/>
-      <c r="S55" s="27"/>
-      <c r="T55" s="27"/>
-      <c r="U55" s="27"/>
-      <c r="V55" s="27"/>
-      <c r="W55" s="27"/>
-      <c r="X55" s="27"/>
-      <c r="Y55" s="27"/>
-      <c r="Z55" s="27"/>
-      <c r="AA55" s="27"/>
-      <c r="AB55" s="27"/>
-      <c r="AC55" s="27"/>
-      <c r="AD55" s="27"/>
-      <c r="AE55" s="27"/>
-      <c r="AF55" s="27"/>
-      <c r="AG55" s="27"/>
-      <c r="AH55" s="27"/>
-    </row>
-    <row r="56" spans="1:34" s="50" customFormat="1" ht="12.75">
-      <c r="I56" s="76"/>
-    </row>
-    <row r="57" spans="1:34" s="50" customFormat="1" ht="12.75"/>
-    <row r="58" spans="1:34" s="50" customFormat="1" ht="12.75"/>
-    <row r="59" spans="1:34" s="50" customFormat="1" ht="12.75"/>
-    <row r="60" spans="1:34" s="50" customFormat="1" ht="12.75"/>
-    <row r="61" spans="1:34" s="50" customFormat="1" ht="12.75"/>
-    <row r="62" spans="1:34" s="50" customFormat="1" ht="12.75"/>
-    <row r="63" spans="1:34" s="50" customFormat="1" ht="12.75"/>
-    <row r="64" spans="1:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="50" spans="9:34" s="50" customFormat="1" ht="12.75">
+      <c r="I50" s="51"/>
+    </row>
+    <row r="51" spans="9:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="52" spans="9:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="53" spans="9:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="54" spans="9:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="55" spans="9:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="56" spans="9:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="57" spans="9:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="58" spans="9:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="59" spans="9:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="60" spans="9:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="61" spans="9:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="62" spans="9:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="63" spans="9:34" s="50" customFormat="1" ht="12.75"/>
+    <row r="64" spans="9:34" s="50" customFormat="1" ht="12.75"/>
     <row r="65" s="50" customFormat="1" ht="12.75"/>
     <row r="66" s="50" customFormat="1" ht="12.75"/>
     <row r="67" s="50" customFormat="1" ht="12.75"/>
@@ -3982,31 +3378,25 @@
     <row r="241" s="50" customFormat="1" ht="12.75"/>
     <row r="242" s="50" customFormat="1" ht="12.75"/>
     <row r="243" s="50" customFormat="1" ht="12.75"/>
-    <row r="244" s="50" customFormat="1" ht="12.75"/>
-    <row r="245" s="50" customFormat="1" ht="12.75"/>
-    <row r="246" s="50" customFormat="1" ht="12.75"/>
-    <row r="247" s="50" customFormat="1" ht="12.75"/>
-    <row r="248" s="50" customFormat="1" ht="12.75"/>
-    <row r="249" s="50" customFormat="1" ht="12.75"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="G34:H34"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="H6:H8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="G27:H27"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A25:C25"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="G34:H34"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="10" orientation="portrait" r:id="rId1"/>

</xml_diff>